<commit_message>
small changes to content and also only prompts user to review topics from most current module
</commit_message>
<xml_diff>
--- a/inst/Data_Analysis_Modules/Module2.xlsx
+++ b/inst/Data_Analysis_Modules/Module2.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
   <si>
     <t>Choices</t>
   </si>
@@ -69,9 +69,6 @@
     <t>command</t>
   </si>
   <si>
-    <t>exact</t>
-  </si>
-  <si>
     <t>Tag</t>
   </si>
   <si>
@@ -126,12 +123,6 @@
     <t xml:space="preserve">In conclusion, three important measures of variability are which of the following: </t>
   </si>
   <si>
-    <t>1. mean, median, range
-2. spread, mean, central tendency
-3. variance, dispersion, spread 
-4. range, variance, standard deviation</t>
-  </si>
-  <si>
     <t>central tendency, dispersion</t>
   </si>
   <si>
@@ -159,9 +150,6 @@
     <t>Type in 'sd(cars$price)' and press enter.</t>
   </si>
   <si>
-    <t>Variance is the standard deviation squared.</t>
-  </si>
-  <si>
     <t>http://youtu.be/E4HAYd0QnRc</t>
   </si>
   <si>
@@ -181,6 +169,18 @@
   </si>
   <si>
     <t xml:space="preserve">Therefore, it is important to describe both the __________ and _________ of a data set. </t>
+  </si>
+  <si>
+    <t>mean, median, range
+spread, mean, central tendency
+variance, dispersion, spread 
+range, variance, standard deviation</t>
+  </si>
+  <si>
+    <t>var(cars$price)</t>
+  </si>
+  <si>
+    <t>Type in 'var(cars$price)' and press enter.</t>
   </si>
 </sst>
 </file>
@@ -330,7 +330,595 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="132">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -950,7 +1538,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -998,7 +1586,7 @@
         <v>3</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>4</v>
@@ -1009,7 +1597,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="9"/>
@@ -1017,7 +1605,7 @@
       <c r="F2" s="10"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1025,7 +1613,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
@@ -1033,7 +1621,7 @@
       <c r="F3" s="10"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1041,7 +1629,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
@@ -1049,7 +1637,7 @@
       <c r="F4" s="10"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
@@ -1057,21 +1645,21 @@
         <v>11</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
@@ -1079,7 +1667,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="11"/>
@@ -1087,7 +1675,7 @@
       <c r="F6" s="9"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
@@ -1095,7 +1683,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="9"/>
@@ -1103,7 +1691,7 @@
       <c r="F7" s="10"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1111,7 +1699,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
@@ -1119,7 +1707,7 @@
       <c r="F8" s="10"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -1127,21 +1715,21 @@
         <v>11</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1149,21 +1737,21 @@
         <v>11</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="11">
         <v>54.5</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1171,7 +1759,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="11"/>
@@ -1179,7 +1767,7 @@
       <c r="F11" s="10"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
@@ -1187,7 +1775,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="11"/>
@@ -1195,7 +1783,7 @@
       <c r="F12" s="10"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1203,7 +1791,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
@@ -1211,7 +1799,7 @@
       <c r="F13" s="10"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
@@ -1219,7 +1807,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="11"/>
@@ -1227,7 +1815,7 @@
       <c r="F14" s="10"/>
       <c r="I14" s="7"/>
       <c r="J14" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1235,21 +1823,21 @@
         <v>11</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
@@ -1257,21 +1845,21 @@
         <v>11</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="11"/>
-      <c r="E16" s="11">
-        <v>132.39840000000001</v>
+      <c r="E16" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -1279,17 +1867,17 @@
         <v>13</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="I17" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
@@ -1297,7 +1885,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
@@ -1305,31 +1893,31 @@
       <c r="F18" s="10"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1781,156 +2369,156 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:J1 A2:A3 C2:J3 A4:J5 A12:J12 A6:A7 C6:J7 A15:J15 A13:A14 C13:J14 A16 C16:J16 A20 C9:J11 A9:A11 A19:C19 E19:J20 C20 A22:J1048576 A21:E21 G21:J21 A17:J18">
-    <cfRule type="expression" dxfId="47" priority="41">
+    <cfRule type="expression" dxfId="87" priority="37">
       <formula>EXACT($A1,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="46">
+    <cfRule type="expression" dxfId="86" priority="38">
       <formula>EXACT($A1,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="47">
+    <cfRule type="expression" dxfId="85" priority="39">
       <formula>EXACT($A1,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="48">
+    <cfRule type="expression" dxfId="84" priority="40">
       <formula>EXACT($A1,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="expression" dxfId="43" priority="37">
+    <cfRule type="expression" dxfId="79" priority="33">
       <formula>EXACT($A2,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="38">
+    <cfRule type="expression" dxfId="78" priority="34">
       <formula>EXACT($A2,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="39">
+    <cfRule type="expression" dxfId="77" priority="35">
       <formula>EXACT($A2,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="40">
+    <cfRule type="expression" dxfId="76" priority="36">
       <formula>EXACT($A2,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="39" priority="33">
+    <cfRule type="expression" dxfId="71" priority="29">
       <formula>EXACT($A6,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="34">
+    <cfRule type="expression" dxfId="70" priority="30">
       <formula>EXACT($A6,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="35">
+    <cfRule type="expression" dxfId="69" priority="31">
       <formula>EXACT($A6,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="36">
+    <cfRule type="expression" dxfId="68" priority="32">
       <formula>EXACT($A6,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="35" priority="25">
+    <cfRule type="expression" dxfId="63" priority="25">
       <formula>EXACT($A7,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="26">
+    <cfRule type="expression" dxfId="62" priority="26">
       <formula>EXACT($A7,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="27">
+    <cfRule type="expression" dxfId="61" priority="27">
       <formula>EXACT($A7,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="28">
+    <cfRule type="expression" dxfId="60" priority="28">
       <formula>EXACT($A7,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:B11">
-    <cfRule type="expression" dxfId="31" priority="21">
+    <cfRule type="expression" dxfId="55" priority="21">
       <formula>EXACT($A9,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="22">
+    <cfRule type="expression" dxfId="54" priority="22">
       <formula>EXACT($A9,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="23">
+    <cfRule type="expression" dxfId="53" priority="23">
       <formula>EXACT($A9,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="24">
+    <cfRule type="expression" dxfId="52" priority="24">
       <formula>EXACT($A9,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B14">
-    <cfRule type="expression" dxfId="27" priority="17">
+    <cfRule type="expression" dxfId="47" priority="17">
       <formula>EXACT($A13,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="18">
+    <cfRule type="expression" dxfId="46" priority="18">
       <formula>EXACT($A13,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="19">
+    <cfRule type="expression" dxfId="45" priority="19">
       <formula>EXACT($A13,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="20">
+    <cfRule type="expression" dxfId="44" priority="20">
       <formula>EXACT($A13,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="23" priority="13">
+    <cfRule type="expression" dxfId="39" priority="13">
       <formula>EXACT($A16,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="14">
+    <cfRule type="expression" dxfId="38" priority="14">
       <formula>EXACT($A16,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="15">
+    <cfRule type="expression" dxfId="37" priority="15">
       <formula>EXACT($A16,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="16">
+    <cfRule type="expression" dxfId="36" priority="16">
       <formula>EXACT($A16,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="expression" dxfId="19" priority="9">
+    <cfRule type="expression" dxfId="31" priority="9">
       <formula>EXACT($A20,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="10">
+    <cfRule type="expression" dxfId="30" priority="10">
       <formula>EXACT($A20,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="11">
+    <cfRule type="expression" dxfId="29" priority="11">
       <formula>EXACT($A20,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="12">
+    <cfRule type="expression" dxfId="28" priority="12">
       <formula>EXACT($A20,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8 C8:J8">
-    <cfRule type="expression" dxfId="15" priority="5">
+    <cfRule type="expression" dxfId="23" priority="5">
       <formula>EXACT($A8,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="6">
+    <cfRule type="expression" dxfId="22" priority="6">
       <formula>EXACT($A8,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="21" priority="7">
       <formula>EXACT($A8,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="20" priority="8">
       <formula>EXACT($A8,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>EXACT($A8,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>EXACT($A8,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>EXACT($A8,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>EXACT($A8,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="7" priority="53">
+    <cfRule type="expression" dxfId="7" priority="41">
       <formula>EXACT($A20,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="54">
+    <cfRule type="expression" dxfId="6" priority="42">
       <formula>EXACT($A20,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="55">
+    <cfRule type="expression" dxfId="5" priority="43">
       <formula>EXACT($A20,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="56">
+    <cfRule type="expression" dxfId="4" priority="44">
       <formula>EXACT($A20,"figure")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
significant upgrades - logs course and module in progress log. only downside is admin function is not working but we will fix on next commit
</commit_message>
<xml_diff>
--- a/inst/Data_Analysis_Modules/Module2.xlsx
+++ b/inst/Data_Analysis_Modules/Module2.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Dropbox\R_Working_Directory\My_Packages\swirl\inst\Data_Analysis_Modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16320" windowHeight="8655"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,12 +17,17 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A:$K</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
   <si>
     <t>Choices</t>
   </si>
@@ -75,48 +80,21 @@
     <t xml:space="preserve">While measures of central tendency are used to estimate the middle values of a dataset, measures of dispersion are important for describing the spread of the data. </t>
   </si>
   <si>
-    <t>The term dispersion refers to degree to which the data values are scattered around an average value.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Two different samples may have the same mean or median, but different levels of variability or vice versa. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">In this module, we will discuss the three statistical values most commonly used to describe the variability of a data set. Variability is a fancy term used to classify how variable or spread out the data is. </t>
-  </si>
-  <si>
     <t xml:space="preserve">The first descriptive statistic that can describe the variability of a data set is known as the RANGE. The range is the difference between the maximum and minimum values of the data set. </t>
   </si>
   <si>
     <t xml:space="preserve">To demonstrate how you can use R to determine the range of a data set we will refer back to the cars data set from the previous module. </t>
   </si>
   <si>
-    <t>The second and third important measures of variability are known as VARIANCE and STANDARD DEVIATION and are very closely related.</t>
-  </si>
-  <si>
-    <t>Mathematically, VARIANCE is the average of the squared differences from the mean. More simply, variance represents the total distance of the data from the mean.</t>
-  </si>
-  <si>
-    <t>The standard deviation can be calculated by taking the square root of the variance and vice versa.</t>
-  </si>
-  <si>
     <t>To Statisticians, the standard deviation is a more conventional measure of variability because it is expressed in the same units as the original data values.</t>
   </si>
   <si>
-    <t>A low value for variance indicates that the data points tend to be located near the mean value; a high value for variance indicates that the data points are spread further from the mean.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Type in the R-command 'range(cars$price)' to determine the exact values for the minimum and maximum prices of cars in the data set. </t>
   </si>
   <si>
     <t xml:space="preserve">Now that you have the minimum and maximum price values, calculate the range of this data. </t>
   </si>
   <si>
-    <t>Use the R-command 'sd(cars$price)' to calculate the standard deviation of the car prices.</t>
-  </si>
-  <si>
-    <t>Now that you have calculated the standard deviation of this data, calculate the variance of the data.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Would you like to watch a short video that goes deeper into how variance and standard deviation are calculated? </t>
   </si>
   <si>
@@ -141,15 +119,9 @@
     <t>The first term refers to the middle of a dataset. The second term refers to the spread of a dataset.</t>
   </si>
   <si>
-    <t xml:space="preserve">Type in 'range(cars$price) without quotations' and hit enter to see the minimum and maximum prices. </t>
-  </si>
-  <si>
     <t>Subtract the minimum price value from the maximum price value.</t>
   </si>
   <si>
-    <t>Type in 'sd(cars$price)' and press enter.</t>
-  </si>
-  <si>
     <t>http://youtu.be/E4HAYd0QnRc</t>
   </si>
   <si>
@@ -178,17 +150,205 @@
   </si>
   <si>
     <t>mean, median, range; spread, mean, central tendency; variance, dispersion, spread; range, variance, standard deviation</t>
+  </si>
+  <si>
+    <t>median, variability; central tendency, dispersion; middle, mean; spread, variability</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The values for variance and standard deviation are very closely related. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The standard deviation can be calculated by taking the square root of the variance </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">where as the variance can be calculated by squaring the standard deviation. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">In R, you can use the command 'var(data)' to easily calculate the variance of a particular set of data. Try calculating the variance for the data 'cars$price'. </t>
+  </si>
+  <si>
+    <t>Similar to variance, you can use the R-command 'sd(data)' to calculate the standard deviation of a particular set of data. Try calculating the standard deviation for the data 'cars$price'.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Type in 'sd(cars$price)' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>without quotations and press enter to see the dtandard deviation of the prices of cars.</t>
+    </r>
+  </si>
+  <si>
+    <t>Type in 'var(cars$price)' without quotations and press enter to see the variance of the prices of cars.</t>
+  </si>
+  <si>
+    <r>
+      <t>Type in 'range(cars$price)'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> without quotation' and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>press</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> enter to see the minimum and maximum prices. </t>
+    </r>
+  </si>
+  <si>
+    <t>exact</t>
+  </si>
+  <si>
+    <t>Welcome to Module 2! In this module, we will learn what DISPERSION is and what statistical values are needed in order to best describe the spread of data.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Why is it important to analyze the spread of a particular set of data? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Two different samples may have the same mean or median, but different levels of variability or vice versa. </t>
+    </r>
+  </si>
+  <si>
+    <t>The second important mesaure of variability is known as VARIANCE. Mathematically, VARIANCE is the average of the squared differences from the mean. More simply, variance represents the total distance of the data from the mean.</t>
+  </si>
+  <si>
+    <t>The term dispersion refers to degree to which the data values are scattered around an average value. Dispersion is synonymous with other words such as variability and the spread.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In this module, we will discuss the three statistical values most commonly used to describe the dispersion or variability of a data set. Variability is a fancy term used to classify how variable or spread out the data is. </t>
+  </si>
+  <si>
+    <r>
+      <t>Using the relationship between standard deviation and variance described above</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">use a different method and your standard deviation value calculated in the previous question to find the variance. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The value for variance is important when later analyzing our data set. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A low value for variance indicates that the data points tend to be located near the mean value; a high value for variance indicates that the data points are spread further from the mean.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculating the range, variance, and standard deviaiton of a data set allows you to more clearly describe the spread of a particular data set. When applied in the real world, lower values for these three statistics will indicate more consistent data wheras higher values for these three statistics will indicate more variable and less consistent data. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -227,8 +387,20 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,6 +425,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -264,126 +442,92 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
-  <dxfs count="44">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="36">
     <dxf>
       <fill>
         <patternFill>
@@ -692,7 +836,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -727,7 +871,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -915,22 +1059,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P130"/>
+  <dimension ref="A1:P126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="75.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="34.28515625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="32.5703125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="32.42578125" style="1" customWidth="1"/>
     <col min="9" max="10" width="33" style="4" customWidth="1"/>
     <col min="11" max="11" width="57.140625" style="2" customWidth="1"/>
     <col min="12" max="12" width="28.7109375" style="1" hidden="1" customWidth="1"/>
@@ -973,386 +1117,397 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:11" s="13" customFormat="1" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="10"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>17</v>
+      <c r="B3" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>18</v>
+      <c r="B4" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>38</v>
-      </c>
+      <c r="B5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+        <v>11</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="10"/>
+      <c r="B7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>21</v>
+      <c r="B8" s="10" t="s">
+        <v>17</v>
       </c>
       <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>39</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>28</v>
+      <c r="B10" s="10" t="s">
+        <v>20</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11">
-        <v>54.5</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>40</v>
+        <v>14</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="10"/>
+        <v>11</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10">
+        <v>54.5</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>23</v>
+      <c r="B12" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="C12" s="10"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="10"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>25</v>
+      <c r="B14" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="10"/>
-      <c r="I14" s="7"/>
+      <c r="I14" s="1"/>
       <c r="J14" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I15" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="I15" s="7"/>
       <c r="J15" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>30</v>
+      <c r="B16" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>50</v>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="I17" s="12" t="s">
-        <v>42</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10">
+        <v>132.39840000000001</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="1"/>
       <c r="J17" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>26</v>
+      <c r="B18" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="C18" s="10"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="78.75" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="I19" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F20" s="11"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="I21" s="11"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F22" s="10"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F23" s="11"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="1:11" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="17"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
@@ -1432,7 +1587,7 @@
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
     </row>
-    <row r="52" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="9:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
@@ -1448,7 +1603,7 @@
       <c r="I55" s="1"/>
       <c r="J55" s="1"/>
     </row>
-    <row r="56" spans="9:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I56" s="1"/>
       <c r="J56" s="1"/>
     </row>
@@ -1532,7 +1687,7 @@
       <c r="I76" s="1"/>
       <c r="J76" s="1"/>
     </row>
-    <row r="77" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="9:10" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I77" s="1"/>
       <c r="J77" s="1"/>
     </row>
@@ -1548,7 +1703,7 @@
       <c r="I80" s="1"/>
       <c r="J80" s="1"/>
     </row>
-    <row r="81" spans="9:10" ht="133.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I81" s="1"/>
       <c r="J81" s="1"/>
     </row>
@@ -1585,14 +1740,14 @@
       <c r="J89" s="1"/>
     </row>
     <row r="90" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
+      <c r="I90" s="3"/>
+      <c r="J90" s="3"/>
     </row>
     <row r="91" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I91" s="1"/>
       <c r="J91" s="1"/>
     </row>
-    <row r="92" spans="9:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="9:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I92" s="1"/>
       <c r="J92" s="1"/>
     </row>
@@ -1601,14 +1756,14 @@
       <c r="J93" s="1"/>
     </row>
     <row r="94" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I94" s="3"/>
-      <c r="J94" s="3"/>
+      <c r="I94" s="1"/>
+      <c r="J94" s="1"/>
     </row>
     <row r="95" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I95" s="1"/>
       <c r="J95" s="1"/>
     </row>
-    <row r="96" spans="9:10" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I96" s="1"/>
       <c r="J96" s="1"/>
     </row>
@@ -1732,181 +1887,142 @@
       <c r="I126" s="1"/>
       <c r="J126" s="1"/>
     </row>
-    <row r="127" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I127" s="1"/>
-      <c r="J127" s="1"/>
-    </row>
-    <row r="128" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I128" s="1"/>
-      <c r="J128" s="1"/>
-    </row>
-    <row r="129" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I129" s="1"/>
-      <c r="J129" s="1"/>
-    </row>
-    <row r="130" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I130" s="1"/>
-      <c r="J130" s="1"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:J1 A2:A3 C2:J3 A4:J5 A12:J12 A6:A7 C6:J7 A15:J15 A13:A14 C13:J14 A16 C16:J16 A20 C9:J11 A9:A11 A19:C19 E19:J20 C20 A22:J1048576 A21:E21 G21:J21 A17:J18">
-    <cfRule type="expression" dxfId="43" priority="37">
+  <conditionalFormatting sqref="A1:J2 A3:A4 C3:J4 A5:J6 A7:A8 C7:J8 A17 C17:J17 A10:J16 A18:J19 A22:D22 A23:J1048576 A21:C21 A20:B20 D20">
+    <cfRule type="expression" dxfId="35" priority="37">
       <formula>EXACT($A1,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="38">
+    <cfRule type="expression" dxfId="34" priority="38">
       <formula>EXACT($A1,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="39">
+    <cfRule type="expression" dxfId="33" priority="39">
       <formula>EXACT($A1,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="40">
+    <cfRule type="expression" dxfId="32" priority="40">
       <formula>EXACT($A1,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="expression" dxfId="39" priority="33">
-      <formula>EXACT($A2,"text")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="34">
-      <formula>EXACT($A2,"video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="35">
-      <formula>EXACT($A2,"question")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="36">
-      <formula>EXACT($A2,"figure")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="35" priority="29">
-      <formula>EXACT($A6,"text")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="30">
-      <formula>EXACT($A6,"video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="31">
-      <formula>EXACT($A6,"question")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="32">
-      <formula>EXACT($A6,"figure")</formula>
+  <conditionalFormatting sqref="B3:B4">
+    <cfRule type="expression" dxfId="31" priority="33">
+      <formula>EXACT($A3,"text")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="34">
+      <formula>EXACT($A3,"video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="35">
+      <formula>EXACT($A3,"question")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="36">
+      <formula>EXACT($A3,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="expression" dxfId="31" priority="25">
+    <cfRule type="expression" dxfId="27" priority="29">
       <formula>EXACT($A7,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="26">
+    <cfRule type="expression" dxfId="26" priority="30">
       <formula>EXACT($A7,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="27">
+    <cfRule type="expression" dxfId="25" priority="31">
       <formula>EXACT($A7,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="28">
+    <cfRule type="expression" dxfId="24" priority="32">
       <formula>EXACT($A7,"figure")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9:B11">
-    <cfRule type="expression" dxfId="27" priority="21">
-      <formula>EXACT($A9,"text")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="22">
-      <formula>EXACT($A9,"video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="23">
-      <formula>EXACT($A9,"question")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="24">
-      <formula>EXACT($A9,"figure")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13:B14">
-    <cfRule type="expression" dxfId="23" priority="17">
-      <formula>EXACT($A13,"text")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="18">
-      <formula>EXACT($A13,"video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="19">
-      <formula>EXACT($A13,"question")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="20">
-      <formula>EXACT($A13,"figure")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="19" priority="13">
-      <formula>EXACT($A16,"text")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="14">
-      <formula>EXACT($A16,"video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="15">
-      <formula>EXACT($A16,"question")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="16">
-      <formula>EXACT($A16,"figure")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="expression" dxfId="15" priority="9">
-      <formula>EXACT($A20,"text")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="10">
-      <formula>EXACT($A20,"video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="11">
-      <formula>EXACT($A20,"question")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="12">
-      <formula>EXACT($A20,"figure")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A8 C8:J8">
-    <cfRule type="expression" dxfId="11" priority="5">
-      <formula>EXACT($A8,"text")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6">
-      <formula>EXACT($A8,"video")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="7">
-      <formula>EXACT($A8,"question")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
-      <formula>EXACT($A8,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="23" priority="25">
       <formula>EXACT($A8,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="22" priority="26">
       <formula>EXACT($A8,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="21" priority="27">
       <formula>EXACT($A8,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="20" priority="28">
       <formula>EXACT($A8,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="3" priority="41">
+  <conditionalFormatting sqref="B17">
+    <cfRule type="expression" dxfId="19" priority="13">
+      <formula>EXACT($A17,"text")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="14">
+      <formula>EXACT($A17,"video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="15">
+      <formula>EXACT($A17,"question")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="16">
+      <formula>EXACT($A17,"figure")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9 C9:J9">
+    <cfRule type="expression" dxfId="15" priority="5">
+      <formula>EXACT($A9,"text")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="6">
+      <formula>EXACT($A9,"video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="7">
+      <formula>EXACT($A9,"question")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="8">
+      <formula>EXACT($A9,"figure")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="expression" dxfId="11" priority="1">
+      <formula>EXACT($A9,"text")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="2">
+      <formula>EXACT($A9,"video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="3">
+      <formula>EXACT($A9,"question")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="4">
+      <formula>EXACT($A9,"figure")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20:J21">
+    <cfRule type="expression" dxfId="7" priority="53">
       <formula>EXACT($A20,"text")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="42">
+    <cfRule type="expression" dxfId="6" priority="54">
       <formula>EXACT($A20,"video")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="43">
+    <cfRule type="expression" dxfId="5" priority="55">
       <formula>EXACT($A20,"question")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="44">
+    <cfRule type="expression" dxfId="4" priority="56">
       <formula>EXACT($A20,"figure")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D21">
+    <cfRule type="expression" dxfId="3" priority="65">
+      <formula>EXACT(#REF!,"text")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="66">
+      <formula>EXACT(#REF!,"video")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="67">
+      <formula>EXACT(#REF!,"question")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="68">
+      <formula>EXACT(#REF!,"figure")</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="I17" r:id="rId1"/>
+    <hyperlink ref="I19" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="37" fitToHeight="0" orientation="landscape" r:id="rId2"/>
+  <pageSetup scale="37" fitToHeight="0" orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>